<commit_message>
entityRecognition: Update test log
Signed-off-by: Yahu Gao <gao_yahu@163.com>
</commit_message>
<xml_diff>
--- a/entityRecognition/baseline-bassedGauss/records.xlsx
+++ b/entityRecognition/baseline-bassedGauss/records.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="138">
   <si>
     <t xml:space="preserve">超参数</t>
   </si>
@@ -33,6 +33,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Bert</t>
     </r>
@@ -41,6 +42,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">使用方式</t>
     </r>
@@ -89,14 +91,15 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">对</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bert</t>
@@ -106,6 +109,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的哪些层进行微调</t>
     </r>
@@ -119,14 +123,15 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">第几轮获得最高</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">F1_score</t>
@@ -150,8 +155,8 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
@@ -162,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">总用时</t>
     </r>
@@ -172,6 +178,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实验</t>
     </r>
@@ -180,24 +187,29 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
+    <t xml:space="preserve">同上</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">微调</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bert</t>
@@ -207,14 +219,15 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">最后两个</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Transformer</t>
@@ -224,6 +237,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层</t>
     </r>
@@ -234,6 +248,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">若</t>
     </r>
@@ -242,6 +257,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">f1</t>
     </r>
@@ -250,15 +266,16 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">降低， 则降低学习率，
- 当学习率接近</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">降低， 则降低学习率， 当学习率接近</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -267,6 +284,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">时，重置学习率</t>
     </r>
@@ -294,6 +312,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">第一个</t>
     </r>
@@ -302,6 +321,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">epoch</t>
     </r>
@@ -310,6 +330,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用时</t>
     </r>
@@ -318,6 +339,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">34</t>
     </r>
@@ -326,6 +348,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒， 其余</t>
     </r>
@@ -334,6 +357,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -342,6 +366,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒</t>
     </r>
@@ -352,6 +377,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">本地验证结果比训练结果低</t>
     </r>
@@ -360,6 +386,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.3</t>
     </r>
@@ -368,6 +395,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">， 在第</t>
     </r>
@@ -376,6 +404,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10</t>
     </r>
@@ -384,6 +413,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">轮达到最佳状态</t>
     </r>
@@ -394,6 +424,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实验</t>
     </r>
@@ -402,12 +433,30 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Maxlen = 500</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Maxlen = 500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">， 其它同上</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">9/30</t>
@@ -431,6 +480,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">第一个</t>
     </r>
@@ -439,6 +489,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">epoch</t>
     </r>
@@ -447,6 +498,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用时</t>
     </r>
@@ -455,6 +507,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">34</t>
     </r>
@@ -463,6 +516,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒， 其余</t>
     </r>
@@ -471,6 +525,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">31</t>
     </r>
@@ -479,6 +534,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒</t>
     </r>
@@ -489,6 +545,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">文本最大长度由</t>
     </r>
@@ -497,6 +554,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">250</t>
     </r>
@@ -505,6 +563,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">扩大到</t>
     </r>
@@ -513,6 +572,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">500</t>
     </r>
@@ -521,6 +581,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">提升不是很明显</t>
     </r>
@@ -531,6 +592,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实验</t>
     </r>
@@ -539,12 +601,29 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Maxlen = 80</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Maxlen = 80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">， 其它同上</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">8/30</t>
@@ -569,6 +648,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">第一个</t>
     </r>
@@ -577,6 +657,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">epoch</t>
     </r>
@@ -585,6 +666,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用时</t>
     </r>
@@ -593,6 +675,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">13</t>
     </r>
@@ -601,6 +684,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒， 其余</t>
     </r>
@@ -609,6 +693,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">11</t>
     </r>
@@ -617,6 +702,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">秒</t>
     </r>
@@ -627,6 +713,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">文本最大长度由</t>
     </r>
@@ -635,6 +722,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">250</t>
     </r>
@@ -643,6 +731,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">缩短到</t>
     </r>
@@ -651,6 +740,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">80</t>
     </r>
@@ -659,6 +749,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -667,6 +758,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">F1_Score</t>
     </r>
@@ -675,6 +767,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">明显下降
 可将</t>
@@ -684,6 +777,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">maxlen</t>
     </r>
@@ -692,6 +786,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">固定为</t>
     </r>
@@ -700,6 +795,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">250</t>
     </r>
@@ -710,161 +806,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">实验</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">4</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxlen=250</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">微调</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">bert</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">最后两个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Transformer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">层
-和第一个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Transformer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">层</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">F1: 0.72388
-P : 0.67430
-R : 0.78132
-L : 0.000049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1: 0.69825
-P : 0.64342
-R : 0.76329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./weights/250_30_16_12_2020-10-08_23_09.weights</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">第一个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">epoch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">用时</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">59</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">秒， 其余</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">52</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">秒</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">可尝试将学习率调整为小于</t>
     </r>
@@ -873,6 +815,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.000006</t>
     </r>
@@ -881,6 +824,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">时立刻重置；
 学习率逐步减小， 当</t>
@@ -890,6 +834,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">f1</t>
     </r>
@@ -898,9 +843,1158 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">降低时增大学习率</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">实验</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Maxlen=250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">， 其它同上</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">微调</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">最后两个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">层和第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">层</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">3/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.72956
+P: 0.69365
+R: 0.76939
+L: 0.00010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.69299
+P :0.63703
+R :0.75973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/250_30_16_12_2020-10-09_09_56.weights
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">59</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">模型在第3轮达到最优， 且高于已有实验，设置学习率逐步降低， 再次观察</t>
+  </si>
+  <si>
+    <t xml:space="preserve">微调更多的层，训练效果更好的情况出现的更多
+但本地验证的效果却有所下降， 判断可能是过拟合了</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">学习率逐步将低0.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，当学习率接近</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">时，重置学习率</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73929
+P: 0.69265
+R: 0.79266
+L: 0.000049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.67540
+P :0.63557
+R :0.72055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/250_30_16_12_2020-10-09_10_39.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本地验证结果比训练结果低0.64， 降低学习率</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Learing_rate = 1e-5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">， 
+其它同上</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">7/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73654
+P: 0.67953
+R: 0.80400
+L: 0.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.67874
+P :0.64282
+R :0.71890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/250_30_16_12_2020-10-09_11_32.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本地验证结果比训练结果低0.58， 在达到最高f1时， 学习率达到设置下限， 开始重置学习率；更新学习率策略</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">学习率逐步将低0.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，当学习率接近</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">时， 学习率保持不变</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">24/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73279
+P: 0.67591
+R: 0.80012
+L: 0.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.69480
+P :0.64304
+R :0.75562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/250_30_16_12_2020-10-09_13_00.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本地验证结果比训练结果低0.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">训练中，精度逐渐提升， 召回逐步降低</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73475
+P: 0.67969
+R: 0.79952
+L: 0.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.70401
+P :0.64507
+R :0.77479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.7426
+P:0.6841
+R:0.8120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_14_41.weights
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">61</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">在线测试比本地验证结果高0.4，
+本地测试比训练结果低0.3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">学习率逐步降低的策略可能更好一些</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">分数中， 召回率明显高于准确率</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">添加BiLSTM(500)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.71950
+P: 0.66182
+R: 0.78819
+L: 0.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.68229
+P :0.62589
+R :0.74986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_15_33.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">88</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">实验10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learing_rate = 1e-4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">添加BiLSTM(128)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73556
+P: 0.66506
+R: 0.82279
+L: 0.000049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.68250
+P :0.63613
+R :0.73616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_16_40.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">87</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">实验11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73586
+P: 0.68159
+R: 0.79952
+L: 0.000024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.70258
+P :0.63750
+R :0.78247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.7428
+P :0.6737
+R :0.8275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_19_26.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本地验证结果不达到0.71，当天不进行提交</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实验12</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">微调</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">最后三个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">层</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73173
+P: 0.67927
+R: 0.79296
+L: 0.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.69914
+P :0.65695
+R :0.74712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_21_18.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">63</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">实验13</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">微调</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">最后五个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">层</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73516
+P: 0.67362
+R: 0.80907
+L: 0.000017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.70071
+P :0.63353
+R :0.78384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_22_05.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">68</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">实验14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">微调</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">最后五个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Transformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">层和第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Transformer层</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.73320
+P: 0.66830
+R: 0.81205
+L: 0.000024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.69426
+P :0.63535
+R :0.76521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_30_16_12_2020-10-09_23_01.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余79秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">实验15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Epochs=10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">， 其它同上</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">将最后5个Transformer层的输出的和作为下一层的输入</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1: 0.74112
+P: 0.68117
+R: 0.81265
+L: 0.000012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1:0.70219
+P :0.63612
+R :0.78356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weights/500_10_16_12_2020-10-09_23_36.weights</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">第一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epoch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">用时8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">秒， 其余78秒</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">可尝试对所有的Transformer层的输出进行微调和求和</t>
   </si>
 </sst>
 </file>
@@ -911,11 +2005,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -936,12 +2031,35 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -986,7 +2104,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1040,6 +2158,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,6 +2173,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,6 +2194,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1070,21 +2264,21 @@
   </sheetPr>
   <dimension ref="A1:AMJ176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="29.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="27.09"/>
@@ -1171,174 +2365,514 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="C3" s="0"/>
-      <c r="D3" s="13" t="s">
-        <v>22</v>
+      <c r="D3" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="14" t="s">
         <v>24</v>
       </c>
+      <c r="F3" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="B4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="14" t="s">
-        <v>32</v>
+      <c r="F4" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>40</v>
       </c>
+      <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="G5" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="B6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G18" s="3"/>

</xml_diff>